<commit_message>
New translations all_translatioens.xlsx (Russian)
</commit_message>
<xml_diff>
--- a/Test/ru.xlsx
+++ b/Test/ru.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Identifier</t>
   </si>
@@ -51,6 +51,9 @@
     <t>Text for translation 3</t>
   </si>
   <si>
+    <t>Текст для перевода 3</t>
+  </si>
+  <si>
     <t>Context_4</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
   </si>
   <si>
     <t>Text for translation 5</t>
+  </si>
+  <si>
+    <t>Текст для перевода 5</t>
   </si>
   <si>
     <t>Hallo!</t>
@@ -545,7 +551,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" customHeight="1" ht="13.8">
@@ -553,16 +559,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3">
         <v>32</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" customHeight="1" ht="13.8">
@@ -570,16 +576,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3">
         <v>23</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -646,10 +652,10 @@
         <v>6</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" customHeight="1" ht="15.75">
@@ -669,10 +675,10 @@
         <v>8</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" customHeight="1" ht="15.75">
@@ -689,13 +695,13 @@
         <v>9</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" customHeight="1" ht="15.75">
@@ -703,22 +709,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" customHeight="1" ht="15.75">
@@ -726,22 +732,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" customHeight="1" ht="15.75">

</xml_diff>